<commit_message>
Added test case 'Valid Login'
</commit_message>
<xml_diff>
--- a/TestPlan.xlsx
+++ b/TestPlan.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\JoelJohnson(G10XIND)\Desktop\cypressFramework\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4690A051-7E0A-4DBA-AE01-1C667048B8FE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6821E771-2508-4A5E-B800-F1AE8FB4C938}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2328" yWindow="348" windowWidth="15216" windowHeight="9204" xr2:uid="{F12E7399-85D7-4ED8-8C27-8CECEEF59108}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="29">
   <si>
     <t>Test Plan - Cypress Test Automation Framework on ParaBank Demo Website</t>
   </si>
@@ -50,15 +50,9 @@
     <t>Completion</t>
   </si>
   <si>
-    <t>INDEX PAGE</t>
-  </si>
-  <si>
     <t>Test Name</t>
   </si>
   <si>
-    <t>Valid test register</t>
-  </si>
-  <si>
     <t>Click on Register to open Test Registration Portal, Enter Values and click on register</t>
   </si>
   <si>
@@ -123,6 +117,24 @@
   </si>
   <si>
     <t>Joel</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">INDEX PAGE - </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>https://parabank.parasoft.com/parabank/index.htm</t>
+    </r>
+  </si>
+  <si>
+    <t>Valid Register</t>
   </si>
 </sst>
 </file>
@@ -172,7 +184,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -184,6 +196,9 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -193,6 +208,12 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -532,7 +553,7 @@
   <dimension ref="A1:H15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G4" sqref="G4"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -540,7 +561,7 @@
     <col min="1" max="1" width="10.6640625" customWidth="1"/>
     <col min="2" max="2" width="17.44140625" customWidth="1"/>
     <col min="3" max="3" width="44.77734375" style="1" customWidth="1"/>
-    <col min="4" max="4" width="11.109375" customWidth="1"/>
+    <col min="4" max="4" width="11.109375" style="10" customWidth="1"/>
     <col min="6" max="6" width="7.44140625" customWidth="1"/>
     <col min="7" max="7" width="10.21875" customWidth="1"/>
     <col min="8" max="8" width="11.77734375" customWidth="1"/>
@@ -553,36 +574,37 @@
       <c r="B1" s="3"/>
       <c r="C1" s="3"/>
       <c r="D1" s="3"/>
-      <c r="E1" s="4"/>
-      <c r="F1" s="4"/>
-      <c r="G1" s="4"/>
-      <c r="H1" s="4"/>
+      <c r="E1" s="5"/>
+      <c r="F1" s="5"/>
+      <c r="G1" s="5"/>
+      <c r="H1" s="5"/>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.3">
       <c r="B2" s="2"/>
-      <c r="C2" s="5"/>
-      <c r="D2" s="2"/>
+      <c r="C2" s="6"/>
+      <c r="D2" s="4"/>
       <c r="E2" s="2"/>
       <c r="F2" s="2"/>
       <c r="G2" s="2"/>
       <c r="H2" s="2"/>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="C3" s="5" t="s">
-        <v>4</v>
-      </c>
+      <c r="B3" s="9" t="s">
+        <v>27</v>
+      </c>
+      <c r="C3" s="9"/>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
         <v>1</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C4" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="C4" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="D4" s="2" t="s">
+      <c r="D4" s="4" t="s">
         <v>3</v>
       </c>
     </row>
@@ -591,13 +613,13 @@
         <v>1</v>
       </c>
       <c r="B5" t="s">
-        <v>6</v>
+        <v>28</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="D5" s="7" t="s">
-        <v>28</v>
+        <v>5</v>
+      </c>
+      <c r="D5" s="8" t="s">
+        <v>26</v>
       </c>
     </row>
     <row r="6" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
@@ -605,10 +627,13 @@
         <v>2</v>
       </c>
       <c r="B6" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>9</v>
+        <v>7</v>
+      </c>
+      <c r="D6" s="8" t="s">
+        <v>26</v>
       </c>
     </row>
     <row r="7" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
@@ -616,10 +641,10 @@
         <v>3</v>
       </c>
       <c r="B7" t="s">
-        <v>10</v>
-      </c>
-      <c r="C7" s="6" t="s">
-        <v>11</v>
+        <v>8</v>
+      </c>
+      <c r="C7" s="7" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="8" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
@@ -627,10 +652,10 @@
         <v>4</v>
       </c>
       <c r="B8" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
     </row>
     <row r="9" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
@@ -638,10 +663,10 @@
         <v>5</v>
       </c>
       <c r="B9" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
     </row>
     <row r="10" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
@@ -649,10 +674,10 @@
         <v>6</v>
       </c>
       <c r="B10" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
     </row>
     <row r="11" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
@@ -660,10 +685,10 @@
         <v>7</v>
       </c>
       <c r="B11" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
     </row>
     <row r="12" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
@@ -671,10 +696,10 @@
         <v>8</v>
       </c>
       <c r="B12" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
     </row>
     <row r="13" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
@@ -682,10 +707,10 @@
         <v>9</v>
       </c>
       <c r="B13" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
     </row>
     <row r="14" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
@@ -693,10 +718,10 @@
         <v>10</v>
       </c>
       <c r="B14" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
     </row>
     <row r="15" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
@@ -704,15 +729,16 @@
         <v>11</v>
       </c>
       <c r="B15" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="1">
+  <mergeCells count="2">
     <mergeCell ref="A1:D1"/>
+    <mergeCell ref="B3:C3"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Added test cases 'Invalid Login' and 'Empty Fields'
</commit_message>
<xml_diff>
--- a/TestPlan.xlsx
+++ b/TestPlan.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\JoelJohnson(G10XIND)\Desktop\cypressFramework\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6821E771-2508-4A5E-B800-F1AE8FB4C938}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1EC32DE8-23BB-42D2-831D-A9FEBC49DA6B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2328" yWindow="348" windowWidth="15216" windowHeight="9204" xr2:uid="{F12E7399-85D7-4ED8-8C27-8CECEEF59108}"/>
+    <workbookView xWindow="2628" yWindow="2508" windowWidth="15804" windowHeight="9828" xr2:uid="{F12E7399-85D7-4ED8-8C27-8CECEEF59108}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="29">
   <si>
     <t>Test Plan - Cypress Test Automation Framework on ParaBank Demo Website</t>
   </si>
@@ -184,7 +184,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -196,25 +196,22 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -552,8 +549,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1A241F10-CE92-4232-ABF1-9D91E198EF21}">
   <dimension ref="A1:H15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="G10" sqref="G10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -561,28 +558,28 @@
     <col min="1" max="1" width="10.6640625" customWidth="1"/>
     <col min="2" max="2" width="17.44140625" customWidth="1"/>
     <col min="3" max="3" width="44.77734375" style="1" customWidth="1"/>
-    <col min="4" max="4" width="11.109375" style="10" customWidth="1"/>
+    <col min="4" max="4" width="11.109375" style="7" customWidth="1"/>
     <col min="6" max="6" width="7.44140625" customWidth="1"/>
     <col min="7" max="7" width="10.21875" customWidth="1"/>
     <col min="8" max="8" width="11.77734375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A1" s="3" t="s">
+      <c r="A1" s="8" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="3"/>
-      <c r="C1" s="3"/>
-      <c r="D1" s="3"/>
-      <c r="E1" s="5"/>
-      <c r="F1" s="5"/>
-      <c r="G1" s="5"/>
-      <c r="H1" s="5"/>
+      <c r="B1" s="8"/>
+      <c r="C1" s="8"/>
+      <c r="D1" s="8"/>
+      <c r="E1" s="4"/>
+      <c r="F1" s="4"/>
+      <c r="G1" s="4"/>
+      <c r="H1" s="4"/>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.3">
       <c r="B2" s="2"/>
-      <c r="C2" s="6"/>
-      <c r="D2" s="4"/>
+      <c r="C2" s="5"/>
+      <c r="D2" s="3"/>
       <c r="E2" s="2"/>
       <c r="F2" s="2"/>
       <c r="G2" s="2"/>
@@ -601,10 +598,10 @@
       <c r="B4" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="C4" s="6" t="s">
+      <c r="C4" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="D4" s="4" t="s">
+      <c r="D4" s="3" t="s">
         <v>3</v>
       </c>
     </row>
@@ -618,7 +615,7 @@
       <c r="C5" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="D5" s="8" t="s">
+      <c r="D5" s="6" t="s">
         <v>26</v>
       </c>
     </row>
@@ -632,7 +629,7 @@
       <c r="C6" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="D6" s="8" t="s">
+      <c r="D6" s="6" t="s">
         <v>26</v>
       </c>
     </row>
@@ -643,8 +640,11 @@
       <c r="B7" t="s">
         <v>8</v>
       </c>
-      <c r="C7" s="7" t="s">
+      <c r="C7" s="1" t="s">
         <v>9</v>
+      </c>
+      <c r="D7" s="6" t="s">
+        <v>26</v>
       </c>
     </row>
     <row r="8" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
@@ -656,6 +656,9 @@
       </c>
       <c r="C8" s="1" t="s">
         <v>11</v>
+      </c>
+      <c r="D8" s="6" t="s">
+        <v>26</v>
       </c>
     </row>
     <row r="9" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
added test cases - Forgot Login Info, Register Link, Latest news links
</commit_message>
<xml_diff>
--- a/TestPlan.xlsx
+++ b/TestPlan.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29328"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\JoelJohnson(G10XIND)\Desktop\cypressFramework\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1EC32DE8-23BB-42D2-831D-A9FEBC49DA6B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B038C885-D8E8-4EE0-AF0B-8E59F00A30D4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2628" yWindow="2508" windowWidth="15804" windowHeight="9828" xr2:uid="{F12E7399-85D7-4ED8-8C27-8CECEEF59108}"/>
+    <workbookView xWindow="1476" yWindow="900" windowWidth="13008" windowHeight="9456" xr2:uid="{F12E7399-85D7-4ED8-8C27-8CECEEF59108}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="21">
   <si>
     <t>Test Plan - Cypress Test Automation Framework on ParaBank Demo Website</t>
   </si>
@@ -86,34 +86,7 @@
     <t>Click on "Register"; should go to account registration page.</t>
   </si>
   <si>
-    <t>Main Menu Links</t>
-  </si>
-  <si>
-    <t>Test navigation of "Solutions," "About Us," "Services," "Products," "Locations," and "Admin Page" links in the menu.</t>
-  </si>
-  <si>
-    <t>ATM services links</t>
-  </si>
-  <si>
-    <t>Verify ATM Services options (Withdraw Funds, Transfer Funds, Check Balances, Make Deposits)</t>
-  </si>
-  <si>
-    <t>Online services links</t>
-  </si>
-  <si>
-    <t>Verify Online Services options (Bill Pay, Account History, Transfer Funds)</t>
-  </si>
-  <si>
     <t>Latest news links</t>
-  </si>
-  <si>
-    <t>Verify all links within latest news section navigates to respective pages</t>
-  </si>
-  <si>
-    <t>Footer Links</t>
-  </si>
-  <si>
-    <t>Verify  "Home," "About Us," "Services," "Products," "Locations," "Forum," "Site Map," and "Contact Us" for correct navigation</t>
   </si>
   <si>
     <t>Joel</t>
@@ -135,6 +108,9 @@
   </si>
   <si>
     <t>Valid Register</t>
+  </si>
+  <si>
+    <t>Verify all links within latest news section navigates to respective page</t>
   </si>
 </sst>
 </file>
@@ -547,10 +523,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1A241F10-CE92-4232-ABF1-9D91E198EF21}">
-  <dimension ref="A1:H15"/>
+  <dimension ref="A1:H11"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="G10" sqref="G10"/>
+    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -587,7 +563,7 @@
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.3">
       <c r="B3" s="9" t="s">
-        <v>27</v>
+        <v>18</v>
       </c>
       <c r="C3" s="9"/>
     </row>
@@ -610,13 +586,13 @@
         <v>1</v>
       </c>
       <c r="B5" t="s">
-        <v>28</v>
+        <v>19</v>
       </c>
       <c r="C5" s="1" t="s">
         <v>5</v>
       </c>
       <c r="D5" s="6" t="s">
-        <v>26</v>
+        <v>17</v>
       </c>
     </row>
     <row r="6" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
@@ -630,7 +606,7 @@
         <v>7</v>
       </c>
       <c r="D6" s="6" t="s">
-        <v>26</v>
+        <v>17</v>
       </c>
     </row>
     <row r="7" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
@@ -644,7 +620,7 @@
         <v>9</v>
       </c>
       <c r="D7" s="6" t="s">
-        <v>26</v>
+        <v>17</v>
       </c>
     </row>
     <row r="8" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
@@ -658,7 +634,7 @@
         <v>11</v>
       </c>
       <c r="D8" s="6" t="s">
-        <v>26</v>
+        <v>17</v>
       </c>
     </row>
     <row r="9" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
@@ -671,6 +647,9 @@
       <c r="C9" s="1" t="s">
         <v>13</v>
       </c>
+      <c r="D9" s="6" t="s">
+        <v>17</v>
+      </c>
     </row>
     <row r="10" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A10">
@@ -682,60 +661,22 @@
       <c r="C10" s="1" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="11" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="D10" s="6" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A11">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="B11" t="s">
         <v>16</v>
       </c>
       <c r="C11" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="D11" s="6" t="s">
         <v>17</v>
-      </c>
-    </row>
-    <row r="12" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A12">
-        <v>8</v>
-      </c>
-      <c r="B12" t="s">
-        <v>18</v>
-      </c>
-      <c r="C12" s="1" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="13" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A13">
-        <v>9</v>
-      </c>
-      <c r="B13" t="s">
-        <v>20</v>
-      </c>
-      <c r="C13" s="1" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="14" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A14">
-        <v>10</v>
-      </c>
-      <c r="B14" t="s">
-        <v>22</v>
-      </c>
-      <c r="C14" s="1" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="15" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A15">
-        <v>11</v>
-      </c>
-      <c r="B15" t="s">
-        <v>24</v>
-      </c>
-      <c r="C15" s="1" t="s">
-        <v>25</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added test cases - Create Checking Account
</commit_message>
<xml_diff>
--- a/TestPlan.xlsx
+++ b/TestPlan.xlsx
@@ -8,12 +8,19 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\JoelJohnson(G10XIND)\Desktop\cypressFramework\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B038C885-D8E8-4EE0-AF0B-8E59F00A30D4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BCD47D5A-030F-4B07-9ED3-285EFA89108F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1476" yWindow="900" windowWidth="13008" windowHeight="9456" xr2:uid="{F12E7399-85D7-4ED8-8C27-8CECEEF59108}"/>
+    <workbookView xWindow="3540" yWindow="1068" windowWidth="13008" windowHeight="9456" activeTab="1" xr2:uid="{F12E7399-85D7-4ED8-8C27-8CECEEF59108}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Index" sheetId="1" r:id="rId1"/>
+    <sheet name="Open Account" sheetId="2" r:id="rId2"/>
+    <sheet name="Overview" sheetId="3" r:id="rId3"/>
+    <sheet name="Transfer" sheetId="4" r:id="rId4"/>
+    <sheet name="Bill Pay" sheetId="5" r:id="rId5"/>
+    <sheet name="Find Trans" sheetId="6" r:id="rId6"/>
+    <sheet name="Update Profile" sheetId="7" r:id="rId7"/>
+    <sheet name="Request Loan" sheetId="8" r:id="rId8"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="39">
   <si>
     <t>Test Plan - Cypress Test Automation Framework on ParaBank Demo Website</t>
   </si>
@@ -111,6 +118,84 @@
   </si>
   <si>
     <t>Verify all links within latest news section navigates to respective page</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">OPEN ACCOUNT PAGE - </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>https://parabank.parasoft.com/parabank/openaccount.htm</t>
+    </r>
+  </si>
+  <si>
+    <t>Create Checking Account</t>
+  </si>
+  <si>
+    <t>Choose 'Checking' from the dropdown list and click on 'Open New Account', and verify in Accounts Overview</t>
+  </si>
+  <si>
+    <t>Create Savings Account</t>
+  </si>
+  <si>
+    <t>Choose 'Savings' from the dropdown list and click on 'Open New Account', and verify in Accounts Overview</t>
+  </si>
+  <si>
+    <t>Create Checking Account - Change Existing Account</t>
+  </si>
+  <si>
+    <t>Create Savings Account - Change Existing Account</t>
+  </si>
+  <si>
+    <t>Choose 'Savings' from the dropdown list, choose 2nd option from existing accounts dropdown and click on 'Open New Account', and verify in Accounts Overview</t>
+  </si>
+  <si>
+    <t>Choose 'Checking' from the dropdown list, choose 2nd option from existing accounts dropdown and click on 'Open New Account', and verify in Accounts Overview</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">OVERVIEW PAGE - </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>https://parabank.parasoft.com/parabank/overview.htm</t>
+    </r>
+  </si>
+  <si>
+    <t>Check Account Details</t>
+  </si>
+  <si>
+    <t>Create new account, click on account link, verify account number and account type</t>
+  </si>
+  <si>
+    <t>Verify Activity Period</t>
+  </si>
+  <si>
+    <t>Click on account link, cycle through all elements of the Activity Period dropdown menu, and verify with transaction dates provided after clicking 'Go'</t>
+  </si>
+  <si>
+    <t>Verify Transaction Type - Debit</t>
+  </si>
+  <si>
+    <t>Click on account link, choose Debit from the Account Type Dropdown menu, and verify all tranasactions are of the type Debit after clicking 'Go'</t>
+  </si>
+  <si>
+    <t>Verify Transaction Type - Credit</t>
+  </si>
+  <si>
+    <t>Click on account link, choose Credit from the Account Type Dropdown menu, and verify all tranasactions are of the type Credit after clicking 'Go'</t>
   </si>
 </sst>
 </file>
@@ -134,7 +219,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -144,6 +229,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -160,7 +251,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -188,6 +279,15 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -525,8 +625,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1A241F10-CE92-4232-ABF1-9D91E198EF21}">
   <dimension ref="A1:H11"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="E11" sqref="E11"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -667,7 +767,7 @@
     </row>
     <row r="11" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A11">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="B11" t="s">
         <v>16</v>
@@ -686,4 +786,292 @@
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3F1684C4-7298-40E1-89F6-4D3AC95D1ADA}">
+  <dimension ref="A1:D11"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E7" sqref="E7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="10.6640625" customWidth="1"/>
+    <col min="2" max="2" width="17.44140625" style="12" customWidth="1"/>
+    <col min="3" max="3" width="52.88671875" customWidth="1"/>
+    <col min="4" max="4" width="11.109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A1" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="8"/>
+      <c r="C1" s="8"/>
+      <c r="D1" s="8"/>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B2" s="11"/>
+      <c r="C2" s="5"/>
+      <c r="D2" s="3"/>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B3" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="C3" s="9"/>
+      <c r="D3" s="7"/>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A4" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B4" s="11" t="s">
+        <v>4</v>
+      </c>
+      <c r="C4" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A5">
+        <v>1</v>
+      </c>
+      <c r="B5" s="12" t="s">
+        <v>22</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="D5" s="6" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A6">
+        <v>2</v>
+      </c>
+      <c r="B6" s="12" t="s">
+        <v>24</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="D6" s="10"/>
+    </row>
+    <row r="7" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A7">
+        <v>3</v>
+      </c>
+      <c r="B7" s="12" t="s">
+        <v>26</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="D7" s="10"/>
+    </row>
+    <row r="8" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A8">
+        <v>4</v>
+      </c>
+      <c r="B8" s="12" t="s">
+        <v>27</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="D8" s="10"/>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="C9" s="1"/>
+      <c r="D9" s="10"/>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="C10" s="1"/>
+      <c r="D10" s="10"/>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="C11" s="1"/>
+      <c r="D11" s="10"/>
+    </row>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="A1:D1"/>
+    <mergeCell ref="B3:C3"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4C4491AB-60FA-47EA-8BAA-63DC4B934046}">
+  <dimension ref="A1:D8"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C16" sqref="C16"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="10.6640625" customWidth="1"/>
+    <col min="2" max="2" width="17.44140625" customWidth="1"/>
+    <col min="3" max="3" width="52.88671875" customWidth="1"/>
+    <col min="4" max="4" width="11.109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A1" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="8"/>
+      <c r="C1" s="8"/>
+      <c r="D1" s="8"/>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B2" s="11"/>
+      <c r="C2" s="5"/>
+      <c r="D2" s="3"/>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B3" s="9" t="s">
+        <v>30</v>
+      </c>
+      <c r="C3" s="9"/>
+      <c r="D3" s="7"/>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A4" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B4" s="11" t="s">
+        <v>4</v>
+      </c>
+      <c r="C4" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A5">
+        <v>1</v>
+      </c>
+      <c r="B5" s="12" t="s">
+        <v>31</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="D5" s="10"/>
+    </row>
+    <row r="6" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A6">
+        <v>2</v>
+      </c>
+      <c r="B6" s="12" t="s">
+        <v>33</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="D6" s="10"/>
+    </row>
+    <row r="7" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A7">
+        <v>3</v>
+      </c>
+      <c r="B7" s="12" t="s">
+        <v>35</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="D7" s="10"/>
+    </row>
+    <row r="8" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A8">
+        <v>4</v>
+      </c>
+      <c r="B8" s="12" t="s">
+        <v>37</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="D8" s="10"/>
+    </row>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="A1:D1"/>
+    <mergeCell ref="B3:C3"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FA24ED60-4239-4A9F-97EE-135B6A5DFA36}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9F090FA6-D6C7-47ED-8CD5-37EFC5F99D19}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{394A18AC-44F5-47FF-B31C-EC12980DAE24}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{14EDACEF-FD47-44C4-B53E-CA795BA86705}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView topLeftCell="E1" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C914FD90-65F7-47F5-AC5D-6FAB0F352DC0}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>